<commit_message>
Database connected to Heroku and it's working
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235DDC3E-C0FE-EB41-9A0A-8910F2A8C7A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03EAAEB-2C0C-4C43-AEFC-B5C6C5E999C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="4760" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
+    <workbookView xWindow="49180" yWindow="1340" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,15 +30,6 @@
     <t>title</t>
   </si>
   <si>
-    <t xml:space="preserve">description </t>
-  </si>
-  <si>
-    <t xml:space="preserve">skills </t>
-  </si>
-  <si>
-    <t xml:space="preserve">image </t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -54,9 +45,6 @@
     <t>project</t>
   </si>
   <si>
-    <t xml:space="preserve">date </t>
-  </si>
-  <si>
     <t xml:space="preserve">project 1 was amazing and super easy to do. </t>
   </si>
   <si>
@@ -187,6 +175,18 @@
   </si>
   <si>
     <t>project 6 title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -559,41 +559,41 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -601,28 +601,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -630,31 +630,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -662,28 +662,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -691,28 +691,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -720,28 +720,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -749,31 +749,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the portfolio html
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03EAAEB-2C0C-4C43-AEFC-B5C6C5E999C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8540F7-D15A-E749-97EA-99B0326BF450}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49180" yWindow="1340" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
+    <workbookView xWindow="500" yWindow="2620" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,24 +81,6 @@
     <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 6</t>
   </si>
   <si>
-    <t>project1.png</t>
-  </si>
-  <si>
-    <t>project2.png</t>
-  </si>
-  <si>
-    <t>project3.png</t>
-  </si>
-  <si>
-    <t>project4.png</t>
-  </si>
-  <si>
-    <t>project5.png</t>
-  </si>
-  <si>
-    <t>project6.png</t>
-  </si>
-  <si>
     <t>https://github.com/navroz-lamba/Image-Classifier-using-VGG-19-CNN</t>
   </si>
   <si>
@@ -187,6 +169,24 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>project1</t>
+  </si>
+  <si>
+    <t>project2</t>
+  </si>
+  <si>
+    <t>project3</t>
+  </si>
+  <si>
+    <t>project4</t>
+  </si>
+  <si>
+    <t>project5</t>
+  </si>
+  <si>
+    <t>project6</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,13 +572,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -610,19 +610,19 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -630,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -639,22 +639,22 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -671,19 +671,19 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -691,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -700,19 +700,19 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -729,19 +729,19 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -758,22 +758,22 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the readme.md and license.md
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8540F7-D15A-E749-97EA-99B0326BF450}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4567E50-A6B3-B44D-AD26-70B8B5F477CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="2620" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
+    <workbookView xWindow="50520" yWindow="1880" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,42 +45,6 @@
     <t>project</t>
   </si>
   <si>
-    <t xml:space="preserve">project 1 was amazing and super easy to do. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">project 2 was amazing and super easy to do. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">project 3 was amazing and super easy to do. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">project 4 was amazing and super easy to do. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">project 5 was amazing and super easy to do. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">project 6 was amazing and super easy to do. </t>
-  </si>
-  <si>
-    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 1</t>
-  </si>
-  <si>
-    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 2</t>
-  </si>
-  <si>
-    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 3</t>
-  </si>
-  <si>
-    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 4</t>
-  </si>
-  <si>
-    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 5</t>
-  </si>
-  <si>
-    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL - 6</t>
-  </si>
-  <si>
     <t>https://github.com/navroz-lamba/Image-Classifier-using-VGG-19-CNN</t>
   </si>
   <si>
@@ -141,24 +105,6 @@
     <t>tag 6</t>
   </si>
   <si>
-    <t>project 1 title</t>
-  </si>
-  <si>
-    <t>project 2 title</t>
-  </si>
-  <si>
-    <t>project 3 title</t>
-  </si>
-  <si>
-    <t>project 4 title</t>
-  </si>
-  <si>
-    <t>project 5 title</t>
-  </si>
-  <si>
-    <t>project 6 title</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -186,7 +132,61 @@
     <t>project5</t>
   </si>
   <si>
-    <t>project6</t>
+    <t>Movie Recommender System with Sentiment Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio Website </t>
+  </si>
+  <si>
+    <t>Airbnb in Los Angeles</t>
+  </si>
+  <si>
+    <t>Human Rights First Asylum</t>
+  </si>
+  <si>
+    <t>Image Classifier using VGG-19 CNN</t>
+  </si>
+  <si>
+    <t>Airbus, the new King of the Skies?!</t>
+  </si>
+  <si>
+    <t>Data Storytelling - Airbus v Boeing - How do they compare?</t>
+  </si>
+  <si>
+    <t>Python, Data Wrangling, Data Visualization</t>
+  </si>
+  <si>
+    <t>HTML, CSS, Python, PlotlyDash, Flask, plotly, Supervised Machine Learning</t>
+  </si>
+  <si>
+    <t>Image Classification using Keras VGG-19 transfer learning</t>
+  </si>
+  <si>
+    <t>HTML, CSS, JavaScript, Python, Flask, TensorFlow, Keras</t>
+  </si>
+  <si>
+    <t>Python, FastAPI,  AWS RDS PostgreSQL, AWS Elastic Beanstalk, Scikit-Learn, Docker, Selenium</t>
+  </si>
+  <si>
+    <t>Predicting the nightly rates of Airbnb in Los Angeles depending on the location, property type, number of bedrooms, etc.</t>
+  </si>
+  <si>
+    <t>HRF needs a web tool backed by data science to aggregate data on asylum cases, allow users to explore that data, and predict and visualize how a judge might rule on a specific asylum case as well as what specific elements of an asylum case seem to most impact a favorable or unfavorable ruling</t>
+  </si>
+  <si>
+    <t>This project showcases my data science projects on a deployed website.</t>
+  </si>
+  <si>
+    <t>HTML, CSS, Python, Bootstrap, Flask, PostgreSQL, Heroku</t>
+  </si>
+  <si>
+    <t>HTML, CSS, JavaScript, Python, Bootstrap, Beautiful Soup, Scikit-Learn, Flask, Heroku</t>
+  </si>
+  <si>
+    <t>Content Based Recommender System recommends movies similar to the movie user likes, and analyses the sentiments on the reviews given by the user for that movie.</t>
+  </si>
+  <si>
+    <t>blogpost-1</t>
   </si>
 </sst>
 </file>
@@ -559,10 +559,16 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
+    <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -572,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -590,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -601,28 +607,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -630,31 +636,29 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -662,28 +666,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -691,28 +695,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -720,28 +727,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -749,31 +756,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +791,7 @@
     <hyperlink ref="F6" r:id="rId3" xr:uid="{00B977C2-4C2A-E04A-AE68-DA94FD6C85B1}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
     <hyperlink ref="G7" r:id="rId5" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{C7481309-669B-844B-B5F2-7ECD1D40F846}"/>
+    <hyperlink ref="G5" r:id="rId6" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
debugged the helper.py file
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4567E50-A6B3-B44D-AD26-70B8B5F477CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ED04A7-7EA0-3D4E-84B1-986583181D7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50520" yWindow="1880" windowWidth="20680" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
+    <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>title</t>
   </si>
@@ -51,13 +51,7 @@
     <t>https://github.com/navroz-lamba/Prediciting-Airbnb-prices-in-LA</t>
   </si>
   <si>
-    <t>https://github.com/navroz-lamba/Algos-and-data-structures</t>
-  </si>
-  <si>
     <t>https://github.com/navroz-lamba/Movie-Recommender-System-with-Sentiment-Analysis</t>
-  </si>
-  <si>
-    <t>https://github.com/Kickstarter-Success-Classifier/kickstarter-</t>
   </si>
   <si>
     <t>https://github.com/Lambda-School-Labs/human-rights-first-asylum-ds-a</t>
@@ -559,7 +553,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,6 +561,7 @@
     <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.5" customWidth="1"/>
     <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="67.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -578,13 +573,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -596,7 +591,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -607,28 +602,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -636,29 +631,29 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -666,28 +661,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -695,31 +690,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -727,28 +722,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -756,42 +751,42 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{29F38D2B-3C77-C049-8016-3204D5CAF60A}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{B9E11E54-9859-7D44-9459-A7C3E4EDA45F}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{00B977C2-4C2A-E04A-AE68-DA94FD6C85B1}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
-    <hyperlink ref="G5" r:id="rId6" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{B9E11E54-9859-7D44-9459-A7C3E4EDA45F}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{5445C8E8-E851-6741-A81F-6DCA6556014B}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{8A37421B-8685-304F-9EC0-5B38B16DDDED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added images to the portfolio page
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ED04A7-7EA0-3D4E-84B1-986583181D7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6727B094-0963-C548-A54F-1C322DB9870C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>title</t>
   </si>
@@ -60,9 +60,6 @@
     <t>https://navrozlamba.com/2020/07/29/king-of-the-skies/</t>
   </si>
   <si>
-    <t>https://navrozlamba.com/2020/08/28/predicting-airbnb-prices-in-los-angeles/</t>
-  </si>
-  <si>
     <t>balle 1</t>
   </si>
   <si>
@@ -141,12 +138,6 @@
     <t>Image Classifier using VGG-19 CNN</t>
   </si>
   <si>
-    <t>Airbus, the new King of the Skies?!</t>
-  </si>
-  <si>
-    <t>Data Storytelling - Airbus v Boeing - How do they compare?</t>
-  </si>
-  <si>
     <t>Python, Data Wrangling, Data Visualization</t>
   </si>
   <si>
@@ -180,7 +171,22 @@
     <t>Content Based Recommender System recommends movies similar to the movie user likes, and analyses the sentiments on the reviews given by the user for that movie.</t>
   </si>
   <si>
-    <t>blogpost-1</t>
+    <t>project6</t>
+  </si>
+  <si>
+    <t>Built a narrative around a set of data, and accompanying visualizations to help convey the sense of competition between the two biggest rivalries of all times; Boeing and Airbus.</t>
+  </si>
+  <si>
+    <t>Airbus, the new King of the Skies?! | Data Storytelling</t>
+  </si>
+  <si>
+    <t>https://movies-u-like.herokuapp.com</t>
+  </si>
+  <si>
+    <t>www.navrozlamba.com</t>
+  </si>
+  <si>
+    <t>https://airbnb-la.herokuapp.com/</t>
   </si>
 </sst>
 </file>
@@ -553,7 +559,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,13 +579,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -591,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -602,28 +608,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -631,29 +640,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -661,28 +672,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -690,31 +701,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -722,28 +733,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -751,16 +762,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -769,13 +780,13 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -787,6 +798,8 @@
     <hyperlink ref="G5" r:id="rId4" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{5445C8E8-E851-6741-A81F-6DCA6556014B}"/>
     <hyperlink ref="F2" r:id="rId6" xr:uid="{8A37421B-8685-304F-9EC0-5B38B16DDDED}"/>
+    <hyperlink ref="G2" r:id="rId7" xr:uid="{181D451C-3560-3F42-A920-A37381F6FD1E}"/>
+    <hyperlink ref="G3" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made changes to the layout.html
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6727B094-0963-C548-A54F-1C322DB9870C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC26E7E-DAAA-D044-B9AD-52D2E45F5E7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>title</t>
   </si>
@@ -57,9 +57,6 @@
     <t>https://github.com/Lambda-School-Labs/human-rights-first-asylum-ds-a</t>
   </si>
   <si>
-    <t>https://navrozlamba.com/2020/07/29/king-of-the-skies/</t>
-  </si>
-  <si>
     <t>balle 1</t>
   </si>
   <si>
@@ -187,6 +184,33 @@
   </si>
   <si>
     <t>https://airbnb-la.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>https://lamba-navroz.medium.com/airbus-the-new-king-of-the-skies-64159fb6e95e</t>
+  </si>
+  <si>
+    <t>project7</t>
+  </si>
+  <si>
+    <t>https://github.com/BW-Med-Cab-4/FAST-API-DS-APP</t>
+  </si>
+  <si>
+    <t>https://medical-cannabis.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>balle 7</t>
+  </si>
+  <si>
+    <t>tag 7</t>
+  </si>
+  <si>
+    <t>Python, Vscode, FastAPI, Pandas, Heroku</t>
+  </si>
+  <si>
+    <t>Recommends a medical cannabis strain depending on the medical condition of the patient.</t>
+  </si>
+  <si>
+    <t>Medical Cannabis Recommender System</t>
   </si>
 </sst>
 </file>
@@ -556,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA8CA54-9BF5-0440-A910-2083D490C1AD}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,13 +603,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -597,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -608,31 +632,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -640,31 +664,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -672,28 +696,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -701,31 +725,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -733,28 +757,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -762,31 +786,63 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="2">
+        <v>44014</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -800,6 +856,8 @@
     <hyperlink ref="F2" r:id="rId6" xr:uid="{8A37421B-8685-304F-9EC0-5B38B16DDDED}"/>
     <hyperlink ref="G2" r:id="rId7" xr:uid="{181D451C-3560-3F42-A920-A37381F6FD1E}"/>
     <hyperlink ref="G3" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{B97DE18B-3A5D-FE4C-8277-B72AFF2FCF86}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added project 8 to the portfolio
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC26E7E-DAAA-D044-B9AD-52D2E45F5E7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91539A3F-794F-9344-860C-1748CA2F2057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>title</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Python, Data Wrangling, Data Visualization</t>
   </si>
   <si>
-    <t>HTML, CSS, Python, PlotlyDash, Flask, plotly, Supervised Machine Learning</t>
-  </si>
-  <si>
     <t>Image Classification using Keras VGG-19 transfer learning</t>
   </si>
   <si>
@@ -211,6 +208,30 @@
   </si>
   <si>
     <t>Medical Cannabis Recommender System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kickstarter Success Classifier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preditcts if the kickstarter project will be successful </t>
+  </si>
+  <si>
+    <t>HTML, CSS, Python, PlotlyDash, Flask, plotly, Scikit-Learn</t>
+  </si>
+  <si>
+    <t>HTML, CSS, Python, Scikit-Learn, Tensorflow, Keras, Flask, Heroku</t>
+  </si>
+  <si>
+    <t>project8</t>
+  </si>
+  <si>
+    <t>https://github.com/Kickstarter-Success-Classifier/kickstarter-</t>
+  </si>
+  <si>
+    <t>https://will-it-kickstart.herokuapp.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balle 8 </t>
   </si>
 </sst>
 </file>
@@ -580,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA8CA54-9BF5-0440-A910-2083D490C1AD}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,10 +656,10 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -647,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -667,10 +688,10 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -679,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -699,10 +720,10 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -728,10 +749,10 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -740,7 +761,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -760,10 +781,10 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -786,22 +807,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -818,31 +839,57 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" t="s">
         <v>56</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
       </c>
       <c r="I8" s="2">
         <v>44014</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -858,6 +905,8 @@
     <hyperlink ref="G3" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
     <hyperlink ref="F8" r:id="rId9" xr:uid="{B97DE18B-3A5D-FE4C-8277-B72AFF2FCF86}"/>
     <hyperlink ref="G8" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{32060B67-64F8-2345-992A-CD10594B4BA0}"/>
+    <hyperlink ref="G9" r:id="rId12" xr:uid="{3166930B-A074-BB49-953A-EE863259546C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The protfolio excel file needed to be fixed
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91539A3F-794F-9344-860C-1748CA2F2057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4021CD7-83C9-044B-89B5-40BECF721644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>title</t>
   </si>
@@ -54,9 +54,6 @@
     <t>https://github.com/navroz-lamba/Movie-Recommender-System-with-Sentiment-Analysis</t>
   </si>
   <si>
-    <t>https://github.com/Lambda-School-Labs/human-rights-first-asylum-ds-a</t>
-  </si>
-  <si>
     <t>balle 1</t>
   </si>
   <si>
@@ -232,6 +229,15 @@
   </si>
   <si>
     <t xml:space="preserve">balle 8 </t>
+  </si>
+  <si>
+    <t>https://github.com/navroz-lamba/human-rights-first-asylum-ds-a</t>
+  </si>
+  <si>
+    <t>https://github.com/navroz-lamba/DataStorytelling</t>
+  </si>
+  <si>
+    <t>https://github.com/navroz-lamba/Portfolio-Website</t>
   </si>
 </sst>
 </file>
@@ -604,7 +610,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,13 +630,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -642,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -653,31 +659,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="2">
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -685,31 +691,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
       <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="2">
         <v>43863</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -717,28 +723,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="2">
         <v>43892</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -746,31 +752,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="2">
         <v>43923</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -778,28 +784,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="2">
         <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -807,31 +813,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="2">
         <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -839,31 +845,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" t="s">
         <v>55</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
       </c>
       <c r="I8" s="2">
         <v>44014</v>
       </c>
       <c r="J8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -871,25 +877,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
         <v>61</v>
       </c>
-      <c r="C9" t="s">
-        <v>62</v>
-      </c>
       <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
         <v>64</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" t="s">
         <v>67</v>
-      </c>
-      <c r="H9" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -907,6 +913,8 @@
     <hyperlink ref="G8" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
     <hyperlink ref="F9" r:id="rId11" xr:uid="{32060B67-64F8-2345-992A-CD10594B4BA0}"/>
     <hyperlink ref="G9" r:id="rId12" xr:uid="{3166930B-A074-BB49-953A-EE863259546C}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{00AFFE45-8290-EF42-BFA1-0E5F4B175BE7}"/>
+    <hyperlink ref="F3" r:id="rId14" xr:uid="{E333392C-9412-3A4A-AE10-7B13608C7642}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the order of the projects in the portfolio page
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4021CD7-83C9-044B-89B5-40BECF721644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082AF120-882D-FA4D-82BC-2C6DD2D6F4C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,31 +691,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2">
-        <v>43863</v>
+        <v>43923</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -752,31 +752,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2">
-        <v>43923</v>
+        <v>43953</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -784,28 +781,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I6" s="2">
-        <v>43953</v>
+        <v>43984</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -813,31 +813,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="I7" s="2">
-        <v>43984</v>
+        <v>44014</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -845,31 +845,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="2">
-        <v>44014</v>
-      </c>
-      <c r="J8" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -877,44 +871,50 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="I9" s="2">
+        <v>43863</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{B9E11E54-9859-7D44-9459-A7C3E4EDA45F}"/>
-    <hyperlink ref="F7" r:id="rId2" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{5445C8E8-E851-6741-A81F-6DCA6556014B}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{B9E11E54-9859-7D44-9459-A7C3E4EDA45F}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{5445C8E8-E851-6741-A81F-6DCA6556014B}"/>
     <hyperlink ref="F2" r:id="rId6" xr:uid="{8A37421B-8685-304F-9EC0-5B38B16DDDED}"/>
     <hyperlink ref="G2" r:id="rId7" xr:uid="{181D451C-3560-3F42-A920-A37381F6FD1E}"/>
-    <hyperlink ref="G3" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{B97DE18B-3A5D-FE4C-8277-B72AFF2FCF86}"/>
-    <hyperlink ref="G8" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{32060B67-64F8-2345-992A-CD10594B4BA0}"/>
-    <hyperlink ref="G9" r:id="rId12" xr:uid="{3166930B-A074-BB49-953A-EE863259546C}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{B97DE18B-3A5D-FE4C-8277-B72AFF2FCF86}"/>
+    <hyperlink ref="G7" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
+    <hyperlink ref="F8" r:id="rId11" xr:uid="{32060B67-64F8-2345-992A-CD10594B4BA0}"/>
+    <hyperlink ref="G8" r:id="rId12" xr:uid="{3166930B-A074-BB49-953A-EE863259546C}"/>
     <hyperlink ref="F4" r:id="rId13" xr:uid="{00AFFE45-8290-EF42-BFA1-0E5F4B175BE7}"/>
-    <hyperlink ref="F3" r:id="rId14" xr:uid="{E333392C-9412-3A4A-AE10-7B13608C7642}"/>
+    <hyperlink ref="F9" r:id="rId14" xr:uid="{E333392C-9412-3A4A-AE10-7B13608C7642}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a new project in the portfolio
</commit_message>
<xml_diff>
--- a/database/portfolio_db_en.xlsx
+++ b/database/portfolio_db_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082AF120-882D-FA4D-82BC-2C6DD2D6F4C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0919D1-C076-7F4D-993D-D8DC6A2881CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>title</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Recommends a medical cannabis strain depending on the medical condition of the patient.</t>
   </si>
   <si>
-    <t>Medical Cannabis Recommender System</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kickstarter Success Classifier </t>
   </si>
   <si>
@@ -238,6 +235,24 @@
   </si>
   <si>
     <t>https://github.com/navroz-lamba/Portfolio-Website</t>
+  </si>
+  <si>
+    <t>Medical Cannabis Recommender System | REST API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covid-19 Dashboard | Tableau </t>
+  </si>
+  <si>
+    <t>Interactive dashboard that displays Covid-19 confirmed cases and deaths by location.</t>
+  </si>
+  <si>
+    <t>Tableau</t>
+  </si>
+  <si>
+    <t>project9</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1zSPfgg0vkOJGJCld17M8KfzCRY1Yzb_o/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -607,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA8CA54-9BF5-0440-A910-2083D490C1AD}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,60 +706,53 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2">
-        <v>43923</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>68</v>
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" s="2">
-        <v>43892</v>
+        <v>43923</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -752,28 +760,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I5" s="2">
-        <v>43953</v>
+        <v>43892</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -781,31 +789,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="2">
-        <v>43984</v>
+        <v>43953</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -813,31 +818,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="I7" s="2">
-        <v>44014</v>
+        <v>43984</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -845,25 +850,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="I8" s="2">
+        <v>44014</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -871,50 +882,77 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <v>43863</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{B9E11E54-9859-7D44-9459-A7C3E4EDA45F}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
-    <hyperlink ref="F5" r:id="rId5" xr:uid="{5445C8E8-E851-6741-A81F-6DCA6556014B}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{B9E11E54-9859-7D44-9459-A7C3E4EDA45F}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{D2B12381-7A2C-FC49-92BB-79B1DBBD7D55}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{3DC61F76-C5E2-EC4A-BD05-83407440E495}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{51737EBC-BE7C-804C-94D1-1431E5A699E3}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{5445C8E8-E851-6741-A81F-6DCA6556014B}"/>
     <hyperlink ref="F2" r:id="rId6" xr:uid="{8A37421B-8685-304F-9EC0-5B38B16DDDED}"/>
     <hyperlink ref="G2" r:id="rId7" xr:uid="{181D451C-3560-3F42-A920-A37381F6FD1E}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
-    <hyperlink ref="F7" r:id="rId9" xr:uid="{B97DE18B-3A5D-FE4C-8277-B72AFF2FCF86}"/>
-    <hyperlink ref="G7" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
-    <hyperlink ref="F8" r:id="rId11" xr:uid="{32060B67-64F8-2345-992A-CD10594B4BA0}"/>
-    <hyperlink ref="G8" r:id="rId12" xr:uid="{3166930B-A074-BB49-953A-EE863259546C}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{00AFFE45-8290-EF42-BFA1-0E5F4B175BE7}"/>
-    <hyperlink ref="F9" r:id="rId14" xr:uid="{E333392C-9412-3A4A-AE10-7B13608C7642}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{6364EBB1-72C1-8F4D-A66C-B3BE5D8D30B5}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{B97DE18B-3A5D-FE4C-8277-B72AFF2FCF86}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{54E251FC-C9BD-AC45-B5B3-64CBE6F0BF2F}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{32060B67-64F8-2345-992A-CD10594B4BA0}"/>
+    <hyperlink ref="G9" r:id="rId12" xr:uid="{3166930B-A074-BB49-953A-EE863259546C}"/>
+    <hyperlink ref="F5" r:id="rId13" xr:uid="{00AFFE45-8290-EF42-BFA1-0E5F4B175BE7}"/>
+    <hyperlink ref="F10" r:id="rId14" xr:uid="{E333392C-9412-3A4A-AE10-7B13608C7642}"/>
+    <hyperlink ref="G3" r:id="rId15" xr:uid="{1EF33CD8-CC56-2043-9616-66EC8A8B6D85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>